<commit_message>
new version first commit
</commit_message>
<xml_diff>
--- a/koruza-compute-module-board/Project Outputs for koruza-compute-module-board/BOM/koruza-compute-module-v0_3_1-BOM.xlsx
+++ b/koruza-compute-module-board/Project Outputs for koruza-compute-module-board/BOM/koruza-compute-module-v0_3_1-BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="264">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -744,9 +744,6 @@
   </si>
   <si>
     <t>GBP</t>
-  </si>
-  <si>
-    <t>USD</t>
   </si>
   <si>
     <t>C:\Users\vojislav\Documents\koruza-compute-module\koruza-compute-module-board\koruza-compute-module-board.PrjPcb</t>
@@ -1773,6 +1770,123 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1785,123 +1899,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2986,8 +2983,8 @@
   </sheetPr>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q57" sqref="Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3165,11 +3162,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>42868</v>
+        <v>42943</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>42868.474343981485</v>
+        <v>42943.404449074071</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="20"/>
@@ -3229,47 +3226,47 @@
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
-      <c r="B10" s="119">
+      <c r="B10" s="115">
         <f t="shared" ref="B10:B57" si="0">ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="117" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="121" t="s">
+      <c r="F10" s="117" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="121" t="s">
+      <c r="G10" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="H10" s="122">
+      <c r="H10" s="118">
         <v>1</v>
       </c>
-      <c r="I10" s="123" t="s">
+      <c r="I10" s="119" t="s">
         <v>195</v>
       </c>
-      <c r="J10" s="121" t="s">
-        <v>251</v>
-      </c>
-      <c r="K10" s="124">
+      <c r="J10" s="117" t="s">
+        <v>250</v>
+      </c>
+      <c r="K10" s="120">
         <v>25</v>
       </c>
-      <c r="L10" s="124">
+      <c r="L10" s="120">
         <v>25</v>
       </c>
-      <c r="M10" s="125">
+      <c r="M10" s="121">
         <v>15.38</v>
       </c>
-      <c r="N10" s="125">
+      <c r="N10" s="121">
         <v>384.5</v>
       </c>
-      <c r="O10" s="126" t="s">
+      <c r="O10" s="122" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3347,7 +3344,7 @@
         <v>193</v>
       </c>
       <c r="J12" s="88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K12" s="37">
         <v>100</v>
@@ -3669,7 +3666,7 @@
         <v>193</v>
       </c>
       <c r="J19" s="87" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K19" s="38">
         <v>125</v>
@@ -3689,186 +3686,186 @@
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="52"/>
-      <c r="B20" s="103">
+      <c r="B20" s="99">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="104" t="s">
+      <c r="D20" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="105" t="s">
+      <c r="E20" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="105" t="s">
+      <c r="F20" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="G20" s="105" t="s">
+      <c r="G20" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="H20" s="106">
+      <c r="H20" s="102">
         <v>1</v>
       </c>
-      <c r="I20" s="107" t="s">
+      <c r="I20" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="J20" s="105" t="s">
+      <c r="J20" s="101" t="s">
         <v>204</v>
       </c>
-      <c r="K20" s="108">
+      <c r="K20" s="104">
         <v>25</v>
       </c>
-      <c r="L20" s="108">
+      <c r="L20" s="104">
         <v>125440</v>
       </c>
-      <c r="M20" s="109">
+      <c r="M20" s="105">
         <v>5.4800000000000001E-2</v>
       </c>
-      <c r="N20" s="109">
-        <v>0</v>
-      </c>
-      <c r="O20" s="110" t="s">
+      <c r="N20" s="105">
+        <v>1.25</v>
+      </c>
+      <c r="O20" s="106" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52"/>
-      <c r="B21" s="127">
+      <c r="B21" s="123">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="128" t="s">
+      <c r="C21" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="128" t="s">
+      <c r="D21" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="128" t="s">
+      <c r="E21" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="F21" s="128" t="s">
+      <c r="F21" s="124" t="s">
         <v>148</v>
       </c>
-      <c r="G21" s="128" t="s">
+      <c r="G21" s="124" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="129">
+      <c r="H21" s="125">
         <v>1</v>
       </c>
-      <c r="I21" s="130" t="s">
+      <c r="I21" s="126" t="s">
         <v>193</v>
       </c>
-      <c r="J21" s="128" t="s">
+      <c r="J21" s="124" t="s">
         <v>205</v>
       </c>
-      <c r="K21" s="131">
+      <c r="K21" s="127">
         <v>25</v>
       </c>
-      <c r="L21" s="131">
+      <c r="L21" s="127">
         <v>25</v>
       </c>
-      <c r="M21" s="132">
+      <c r="M21" s="128">
         <v>19.5</v>
       </c>
-      <c r="N21" s="132">
-        <v>0</v>
-      </c>
-      <c r="O21" s="133" t="s">
+      <c r="N21" s="128">
+        <v>487.5</v>
+      </c>
+      <c r="O21" s="129" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52"/>
-      <c r="B22" s="119">
+      <c r="B22" s="115">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="120" t="s">
+      <c r="C22" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="120" t="s">
+      <c r="D22" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="121" t="s">
+      <c r="E22" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="121" t="s">
+      <c r="F22" s="117" t="s">
         <v>166</v>
       </c>
-      <c r="G22" s="121" t="s">
+      <c r="G22" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="H22" s="122">
+      <c r="H22" s="118">
         <v>1</v>
       </c>
-      <c r="I22" s="123" t="s">
+      <c r="I22" s="119" t="s">
         <v>193</v>
       </c>
-      <c r="J22" s="121" t="s">
+      <c r="J22" s="117" t="s">
         <v>206</v>
       </c>
-      <c r="K22" s="124">
+      <c r="K22" s="120">
         <v>25</v>
       </c>
-      <c r="L22" s="124">
+      <c r="L22" s="120">
         <v>76</v>
       </c>
-      <c r="M22" s="125">
+      <c r="M22" s="121">
         <v>28.95</v>
       </c>
-      <c r="N22" s="125">
+      <c r="N22" s="121">
         <v>723.75</v>
       </c>
-      <c r="O22" s="126" t="s">
+      <c r="O22" s="122" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="111">
+      <c r="B23" s="107">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="112" t="s">
+      <c r="C23" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="112" t="s">
+      <c r="D23" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="112" t="s">
+      <c r="E23" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="112" t="s">
+      <c r="F23" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="112" t="s">
+      <c r="G23" s="108" t="s">
         <v>186</v>
       </c>
-      <c r="H23" s="113">
+      <c r="H23" s="109">
         <v>1</v>
       </c>
-      <c r="I23" s="114" t="s">
+      <c r="I23" s="110" t="s">
         <v>194</v>
       </c>
-      <c r="J23" s="112" t="s">
+      <c r="J23" s="108" t="s">
         <v>207</v>
       </c>
-      <c r="K23" s="115">
+      <c r="K23" s="111">
         <v>25</v>
       </c>
-      <c r="L23" s="115">
+      <c r="L23" s="111">
         <v>25</v>
       </c>
-      <c r="M23" s="116">
+      <c r="M23" s="112">
         <v>0.30299999999999999</v>
       </c>
-      <c r="N23" s="116">
-        <v>0</v>
-      </c>
-      <c r="O23" s="117" t="s">
-        <v>259</v>
+      <c r="N23" s="112">
+        <v>7.5</v>
+      </c>
+      <c r="O23" s="113" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4037,7 +4034,7 @@
         <v>193</v>
       </c>
       <c r="J27" s="87" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K27" s="38">
         <v>75</v>
@@ -4313,7 +4310,7 @@
         <v>193</v>
       </c>
       <c r="J33" s="87" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K33" s="38">
         <v>25</v>
@@ -4543,7 +4540,7 @@
         <v>193</v>
       </c>
       <c r="J38" s="88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K38" s="37">
         <v>100</v>
@@ -4747,45 +4744,45 @@
     </row>
     <row r="43" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="52"/>
-      <c r="B43" s="111">
+      <c r="B43" s="107">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C43" s="112" t="s">
+      <c r="C43" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="112" t="s">
+      <c r="D43" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="E43" s="112" t="s">
+      <c r="E43" s="108" t="s">
         <v>143</v>
       </c>
-      <c r="F43" s="112" t="s">
+      <c r="F43" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="G43" s="112" t="s">
+      <c r="G43" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="H43" s="113">
+      <c r="H43" s="109">
         <v>2</v>
       </c>
-      <c r="I43" s="114" t="s">
+      <c r="I43" s="110" t="s">
         <v>193</v>
       </c>
-      <c r="J43" s="112" t="s">
+      <c r="J43" s="108" t="s">
         <v>224</v>
       </c>
-      <c r="K43" s="115">
+      <c r="K43" s="111">
         <v>50</v>
       </c>
-      <c r="L43" s="115">
+      <c r="L43" s="111">
         <v>1629</v>
       </c>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116">
+      <c r="M43" s="112"/>
+      <c r="N43" s="112">
         <v>0</v>
       </c>
-      <c r="O43" s="117" t="s">
+      <c r="O43" s="113" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4860,10 +4857,10 @@
         <v>3</v>
       </c>
       <c r="I45" s="90" t="s">
+        <v>256</v>
+      </c>
+      <c r="J45" s="87" t="s">
         <v>257</v>
-      </c>
-      <c r="J45" s="87" t="s">
-        <v>258</v>
       </c>
       <c r="K45" s="38">
         <v>100</v>
@@ -4883,47 +4880,47 @@
     </row>
     <row r="46" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="52"/>
-      <c r="B46" s="134">
+      <c r="B46" s="130">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C46" s="135" t="s">
+      <c r="C46" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="135" t="s">
+      <c r="D46" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="E46" s="136" t="s">
+      <c r="E46" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="F46" s="136" t="s">
+      <c r="F46" s="132" t="s">
         <v>173</v>
       </c>
-      <c r="G46" s="136" t="s">
+      <c r="G46" s="132" t="s">
         <v>188</v>
       </c>
-      <c r="H46" s="137">
+      <c r="H46" s="133">
         <v>1</v>
       </c>
-      <c r="I46" s="138" t="s">
+      <c r="I46" s="134" t="s">
         <v>194</v>
       </c>
-      <c r="J46" s="136" t="s">
+      <c r="J46" s="132" t="s">
         <v>226</v>
       </c>
-      <c r="K46" s="139">
+      <c r="K46" s="135">
         <v>25</v>
       </c>
-      <c r="L46" s="139">
+      <c r="L46" s="135">
         <v>25</v>
       </c>
-      <c r="M46" s="140">
+      <c r="M46" s="136">
         <v>0.55500000000000005</v>
       </c>
-      <c r="N46" s="140">
-        <v>0</v>
-      </c>
-      <c r="O46" s="141" t="s">
+      <c r="N46" s="136">
+        <v>14</v>
+      </c>
+      <c r="O46" s="137" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4980,19 +4977,19 @@
         <v>39</v>
       </c>
       <c r="C48" s="86" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D48" s="86" t="s">
         <v>90</v>
       </c>
       <c r="E48" s="88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F48" s="88" t="s">
         <v>175</v>
       </c>
       <c r="G48" s="88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H48" s="29">
         <v>2</v>
@@ -5001,7 +4998,7 @@
         <v>193</v>
       </c>
       <c r="J48" s="88" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K48" s="37">
         <v>50</v>
@@ -5010,7 +5007,7 @@
         <v>257</v>
       </c>
       <c r="M48" s="76" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N48" s="76">
         <v>17.7</v>
@@ -5108,52 +5105,52 @@
         <v>106.88</v>
       </c>
       <c r="O50" s="94" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="52"/>
-      <c r="B51" s="127">
+      <c r="B51" s="123">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="C51" s="128" t="s">
+      <c r="C51" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="128" t="s">
+      <c r="D51" s="124" t="s">
         <v>104</v>
       </c>
-      <c r="E51" s="128" t="s">
+      <c r="E51" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="F51" s="128" t="s">
+      <c r="F51" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="G51" s="128" t="s">
+      <c r="G51" s="124" t="s">
         <v>189</v>
       </c>
-      <c r="H51" s="129">
+      <c r="H51" s="125">
         <v>1</v>
       </c>
-      <c r="I51" s="130" t="s">
+      <c r="I51" s="126" t="s">
         <v>194</v>
       </c>
-      <c r="J51" s="128" t="s">
+      <c r="J51" s="124" t="s">
         <v>230</v>
       </c>
-      <c r="K51" s="131">
+      <c r="K51" s="127">
         <v>25</v>
       </c>
-      <c r="L51" s="131">
+      <c r="L51" s="127">
         <v>1438</v>
       </c>
-      <c r="M51" s="132">
+      <c r="M51" s="128">
         <v>4.58</v>
       </c>
-      <c r="N51" s="132">
-        <v>0</v>
-      </c>
-      <c r="O51" s="133" t="s">
+      <c r="N51" s="128">
+        <v>114.5</v>
+      </c>
+      <c r="O51" s="129" t="s">
         <v>242</v>
       </c>
     </row>
@@ -5378,13 +5375,13 @@
         <v>6446</v>
       </c>
       <c r="M56" s="76">
-        <v>4.5</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="N56" s="76">
-        <v>112.5</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="O56" s="94" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5455,16 +5452,16 @@
       <c r="M58" s="42"/>
       <c r="N58" s="42">
         <f>SUM(N10:N57)</f>
-        <v>1911.8419999999999</v>
+        <v>2426.3169999999996</v>
       </c>
       <c r="O58" s="63"/>
     </row>
     <row r="59" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="52"/>
-      <c r="B59" s="99" t="s">
+      <c r="B59" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="99"/>
+      <c r="C59" s="138"/>
       <c r="D59" s="5"/>
       <c r="E59" s="7"/>
       <c r="F59" s="46" t="s">
@@ -5498,11 +5495,11 @@
         <v>23</v>
       </c>
       <c r="K60" s="36"/>
-      <c r="L60" s="100">
+      <c r="L60" s="139">
         <f>N58</f>
-        <v>1911.8419999999999</v>
-      </c>
-      <c r="M60" s="101"/>
+        <v>2426.3169999999996</v>
+      </c>
+      <c r="M60" s="140"/>
       <c r="N60" s="84" t="s">
         <v>242</v>
       </c>
@@ -5522,12 +5519,12 @@
         <v>25</v>
       </c>
       <c r="K61" s="6"/>
-      <c r="L61" s="102">
+      <c r="L61" s="141">
         <f>L60/H60</f>
-        <v>76.473680000000002</v>
-      </c>
-      <c r="M61" s="102"/>
-      <c r="N61" s="118" t="s">
+        <v>97.052679999999981</v>
+      </c>
+      <c r="M61" s="141"/>
+      <c r="N61" s="114" t="s">
         <v>242</v>
       </c>
       <c r="O61" s="62"/>
@@ -6074,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="96" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6106,7 +6103,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6114,7 +6111,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6122,7 +6119,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6146,7 +6143,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6154,7 +6151,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6162,7 +6159,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="97" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -6170,7 +6167,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="98" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6178,7 +6175,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="97" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>